<commit_message>
Updated transcript name format sheet
</commit_message>
<xml_diff>
--- a/TheNewComparativeSet.xlsx
+++ b/TheNewComparativeSet.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6011" uniqueCount="2810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5995" uniqueCount="2794">
   <si>
     <t xml:space="preserve">Num</t>
   </si>
@@ -7537,100 +7537,55 @@
     <t xml:space="preserve">&gt;EP00315_Gephyrocapsa_oceanica_P000001 CAMPEP_0185326042 /NCGR_PEP_ID=MMETSP1363-20130426|67725_1 /TAXON_ID=38817 /ORGANISM="Gephyrocapsa oceanica</t>
   </si>
   <si>
-    <t xml:space="preserve"> Strain RCC1303" /LENGTH=74 /DNA_ID=CAMNT_0027924759 /DNA_START=1 /DNA_END=221 /DNA_ORIENTATION=-</t>
-  </si>
-  <si>
     <t xml:space="preserve">&gt;EP00320_Phaeocystis_rex_P000001 CAMPEP_0119065636 /NCGR_PEP_ID=MMETSP1178-20130426|8405_1 /TAXON_ID=33656 /ORGANISM="unid sp</t>
   </si>
   <si>
-    <t xml:space="preserve"> Strain CCMP2000" /LENGTH=57 /DNA_ID=CAMNT_0007047167 /DNA_START=1 /DNA_END=168 /DNA_ORIENTATION=-</t>
-  </si>
-  <si>
     <t xml:space="preserve">&gt;EP00327_Prymnesium_parvum_P000001 CAMPEP_0182831408 /NCGR_PEP_ID=MMETSP0006_2-20121128|19115_1 /TAXON_ID=97485 /ORGANISM="Prymnesium parvum</t>
   </si>
   <si>
-    <t xml:space="preserve"> Strain Texoma1" /LENGTH=168 /DNA_ID=CAMNT_0024959085 /DNA_START=1 /DNA_END=506 /DNA_ORIENTATION=-</t>
-  </si>
-  <si>
     <t xml:space="preserve">&gt;EP00331_Platyophrya_macrostoma_P000001 CAMPEP_0176405384 /NCGR_PEP_ID=MMETSP0127-20121128|307_1 /TAXON_ID=938130 /ORGANISM="Platyophrya macrostoma</t>
   </si>
   <si>
-    <t xml:space="preserve"> Strain WH" /LENGTH=329 /DNA_ID=CAMNT_0017784435 /DNA_START=57 /DNA_END=1046 /DNA_ORIENTATION=+</t>
-  </si>
-  <si>
     <t xml:space="preserve">&gt;EP00357_Protocruzia_adherens_P000001 CAMPEP_0115000590 /NCGR_PEP_ID=MMETSP0216-20121206|16853_1 /TAXON_ID=223996 /ORGANISM="Protocruzia adherens</t>
   </si>
   <si>
-    <t xml:space="preserve"> Strain Boccale" /LENGTH=313 /DNA_ID=CAMNT_0002365727 /DNA_START=30 /DNA_END=967 /DNA_ORIENTATION=-</t>
-  </si>
-  <si>
     <t xml:space="preserve">&gt;EP00451_Oxyrrhis_marina_P000001 CAMPEP_0204264522 /NCGR_PEP_ID=MMETSP0468-20130131|9078_1 /ASSEMBLY_ACC=CAM_ASM_000383 /TAXON_ID=2969 /ORGANISM="Oxyrrhis marina" /LENGTH=113 /DNA_ID=CAMNT_0051239397 /DNA_START=1 /DNA_END=335 /DNA_ORIENTATION=-</t>
   </si>
   <si>
     <t xml:space="preserve">&gt;EP00462_Mataza_sp_D1_P000001 CAMPEP_0175088676 /NCGR_PEP_ID=MMETSP0086_2-20121207|374_1 /TAXON_ID=136419 /ORGANISM="Unknown Unknown</t>
   </si>
   <si>
-    <t xml:space="preserve"> Strain D1" /LENGTH=316 /DNA_ID=CAMNT_0016361123 /DNA_START=1 /DNA_END=951 /DNA_ORIENTATION=-</t>
-  </si>
-  <si>
     <t xml:space="preserve">&gt;EP00465_Bigelowiella_longifila_P000001 CAMPEP_0185251060 /NCGR_PEP_ID=MMETSP1359-20130426|331_1 /TAXON_ID=552665 /ORGANISM="Bigelowiella longifila</t>
   </si>
   <si>
-    <t xml:space="preserve"> Strain CCMP242" /LENGTH=193 /DNA_ID=CAMNT_0027832767 /DNA_START=1 /DNA_END=582 /DNA_ORIENTATION=+</t>
-  </si>
-  <si>
     <t xml:space="preserve">&gt;EP00468_Gymnochlora_sp_CCMP2014_P000001 CAMPEP_0167740886 /NCGR_PEP_ID=MMETSP0110_2-20121227|543_1 /TAXON_ID=629695 /ORGANISM="Gymnochlora sp.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Strain CCMP2014" /LENGTH=945 /DNA_ID=CAMNT_0007624863 /DNA_START=1 /DNA_END=2834 /DNA_ORIENTATION=-</t>
-  </si>
-  <si>
     <t xml:space="preserve">&gt;EP00469_Lotharella_globosa_P000001 CAMPEP_0167801286 /NCGR_PEP_ID=MMETSP0111_2-20121227|18316_1 /TAXON_ID=91324 /ORGANISM="Lotharella globosa</t>
   </si>
   <si>
-    <t xml:space="preserve"> Strain CCCM811" /LENGTH=54 /DNA_ID=CAMNT_0007696867 /DNA_START=1 /DNA_END=165 /DNA_ORIENTATION=+</t>
-  </si>
-  <si>
     <t xml:space="preserve">&gt;EP00499_Haloplacidia_sp_CaronLabIsolate_P000001 CAMPEP_0196797304 /NCGR_PEP_ID=MMETSP1104-20130614|38569_1 /TAXON_ID=33652 /ORGANISM="Cafeteria sp.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Strain Caron Lab Isolate" /LENGTH=1283 /DNA_ID=CAMNT_0042167709 /DNA_START=1 /DNA_END=3852 /DNA_ORIENTATION=-</t>
-  </si>
-  <si>
     <t xml:space="preserve">&gt;EP00500_Bicosoecida_sp_ms1_P000001 CAMPEP_0203806246 /NCGR_PEP_ID=MMETSP0115-20131106|255_1 /ASSEMBLY_ACC=CAM_ASM_000227 /TAXON_ID=33651 /ORGANISM="Bicosoecid sp</t>
   </si>
   <si>
-    <t xml:space="preserve"> Strain ms1" /LENGTH=879 /DNA_ID=CAMNT_0050714901 /DNA_START=1 /DNA_END=2631 /DNA_ORIENTATION=-</t>
-  </si>
-  <si>
     <t xml:space="preserve">&gt;EP00511_Aplanochytrium_stocchinoi_P000001 CAMPEP_0204822436 /NCGR_PEP_ID=MMETSP1346-20131115|619_1 /ASSEMBLY_ACC=CAM_ASM_000771 /TAXON_ID=215587 /ORGANISM="Aplanochytrium stocchinoi</t>
   </si>
   <si>
-    <t xml:space="preserve"> Strain GSBS06" /LENGTH=312 /DNA_ID=CAMNT_0051948639 /DNA_START=287 /DNA_END=1225 /DNA_ORIENTATION=+</t>
-  </si>
-  <si>
     <t xml:space="preserve">&gt;EP00519_Triparma_laevis_P000001 CAMPEP_0182507824 /NCGR_PEP_ID=MMETSP1321-20130603|23905_1 /TAXON_ID=91990 /ORGANISM="Bolidomonas sp.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Strain RCC1657" /LENGTH=586 /DNA_ID=CAMNT_0024713797 /DNA_START=1 /DNA_END=1760 /DNA_ORIENTATION=+</t>
-  </si>
-  <si>
     <t xml:space="preserve">&gt;EP00592_Proboscia_alata_P000001 CAMPEP_0194366204 /NCGR_PEP_ID=MMETSP0174-20130528|14236_1 /TAXON_ID=216777 /ORGANISM="Proboscia alata</t>
   </si>
   <si>
-    <t xml:space="preserve"> Strain PI-D3" /LENGTH=53 /DNA_ID=CAMNT_0039141267 /DNA_START=1 /DNA_END=157 /DNA_ORIENTATION=+</t>
-  </si>
-  <si>
     <t xml:space="preserve">&gt;EP00638_Chattonella_subsalsa_P000001 CAMPEP_0117759142 /NCGR_PEP_ID=MMETSP0947-20121206|15836_1 /TAXON_ID=44440 /ORGANISM="Chattonella subsalsa</t>
   </si>
   <si>
-    <t xml:space="preserve"> Strain CCMP2191" /LENGTH=177 /DNA_ID=CAMNT_0005579541 /DNA_START=108 /DNA_END=641 /DNA_ORIENTATION=+</t>
-  </si>
-  <si>
     <t xml:space="preserve">&gt;EP00672_Neobodo_designis_P000001 CAMPEP_0174884242 /NCGR_PEP_ID=MMETSP1114-20130205|85670_1 /TAXON_ID=312471 /ORGANISM="Neobodo designis</t>
   </si>
   <si>
-    <t xml:space="preserve"> Strain CCAP 1951/1" /LENGTH=303 /DNA_ID=CAMNT_0016119645 /DNA_START=1 /DNA_END=908 /DNA_ORIENTATION=+</t>
+    <t xml:space="preserve">&gt;EP00818_Percolomonas_sp_WS_P000001 CAMPEP_0117440384 /NCGR_PEP_ID=MMETSP0759-20121206|3064_1 /TAXON_ID=63605 /ORGANISM="Percolomonas cosmopolitus, Strain WS" /LENGTH=121 /DNA_ID=CAMNT_0005232151 /DNA_START=1 /DNA_END=366 /DNA_ORIENTATION=+</t>
   </si>
   <si>
     <t xml:space="preserve">&gt;EP00741_Cyanophora_paradoxa_P000001 tig00000017_g1.t1</t>
@@ -7643,9 +7598,6 @@
   </si>
   <si>
     <t xml:space="preserve">&gt;EP00770_Monocercomonoides_exilis_P000001 MONOS_1.1-p1 | transcript=MONOS_1.1 | gene=MONOS_1 | organism=Monocercomonoides_exilis_PA203 | gene_product=unspecified product | transcript_product=unspecified product | location=Mono_scaffold00001:5945-8323(-) | protein_length=792 | sequence_SO=supercontig | SO=protein_coding | is_pseudo=false</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt;EP00818_Percolomonas_sp_WS_P000001 CAMPEP_0117440384 /NCGR_PEP_ID=MMETSP0759-20121206|3064_1 /TAXON_ID=63605 /ORGANISM="Percolomonas cosmopolitus, Strain WS" /LENGTH=121 /DNA_ID=CAMNT_0005232151 /DNA_START=1 /DNA_END=366 /DNA_ORIENTATION=+</t>
   </si>
   <si>
     <t xml:space="preserve">&gt;EP00820_Chromera_velia_P000001 Cvel_145.t1-p1 | transcript=Cvel_145.t1 | gene=Cvel_145 | organism=Chromera_velia_CCMP2878 | gene_product=hypothetical protein | transcript_product=hypothetical protein | location=Cvel_scaffold10:720-1220(+) | protein_length=167 | sequence_SO=supercontig | SO=protein_coding | is_pseudo=false</t>
@@ -8732,8 +8684,8 @@
   </sheetPr>
   <dimension ref="A1:AI245"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A116" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D191" activeCellId="0" sqref="D191"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P54" activeCellId="0" sqref="P54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27053,7 +27005,7 @@
   </sheetPr>
   <dimension ref="A1:K117"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -32147,8 +32099,8 @@
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A119" activeCellId="0" sqref="A119"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A84" activeCellId="0" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33807,7 +33759,10 @@
       <c r="A83" s="0" t="s">
         <v>2070</v>
       </c>
-      <c r="B83" s="0" t="s">
+      <c r="B83" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C83" s="0" t="s">
         <v>2491</v>
       </c>
     </row>
@@ -33815,7 +33770,7 @@
       <c r="A84" s="0" t="s">
         <v>2072</v>
       </c>
-      <c r="B84" s="0" t="s">
+      <c r="C84" s="0" t="s">
         <v>2492</v>
       </c>
     </row>
@@ -33823,7 +33778,7 @@
       <c r="A85" s="0" t="s">
         <v>2074</v>
       </c>
-      <c r="B85" s="0" t="s">
+      <c r="C85" s="0" t="s">
         <v>2493</v>
       </c>
     </row>
@@ -33831,7 +33786,10 @@
       <c r="A86" s="0" t="s">
         <v>2075</v>
       </c>
-      <c r="B86" s="0" t="s">
+      <c r="B86" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C86" s="0" t="s">
         <v>2494</v>
       </c>
     </row>
@@ -33839,7 +33797,10 @@
       <c r="A87" s="0" t="s">
         <v>2076</v>
       </c>
-      <c r="B87" s="0" t="s">
+      <c r="B87" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C87" s="0" t="s">
         <v>2495</v>
       </c>
     </row>
@@ -33847,7 +33808,10 @@
       <c r="A88" s="0" t="s">
         <v>2077</v>
       </c>
-      <c r="B88" s="0" t="s">
+      <c r="B88" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C88" s="0" t="s">
         <v>2496</v>
       </c>
     </row>
@@ -33855,7 +33819,10 @@
       <c r="A89" s="0" t="s">
         <v>2078</v>
       </c>
-      <c r="B89" s="0" t="s">
+      <c r="B89" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C89" s="0" t="s">
         <v>2497</v>
       </c>
     </row>
@@ -33863,7 +33830,10 @@
       <c r="A90" s="0" t="s">
         <v>2079</v>
       </c>
-      <c r="B90" s="0" t="s">
+      <c r="B90" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C90" s="0" t="s">
         <v>2498</v>
       </c>
     </row>
@@ -33871,7 +33841,10 @@
       <c r="A91" s="0" t="s">
         <v>2080</v>
       </c>
-      <c r="B91" s="0" t="s">
+      <c r="B91" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C91" s="0" t="s">
         <v>2499</v>
       </c>
     </row>
@@ -33879,7 +33852,10 @@
       <c r="A92" s="0" t="s">
         <v>2081</v>
       </c>
-      <c r="B92" s="0" t="s">
+      <c r="B92" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C92" s="0" t="s">
         <v>2500</v>
       </c>
     </row>
@@ -33887,7 +33863,10 @@
       <c r="A93" s="0" t="s">
         <v>2082</v>
       </c>
-      <c r="B93" s="0" t="s">
+      <c r="B93" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C93" s="0" t="s">
         <v>2500</v>
       </c>
     </row>
@@ -33895,7 +33874,10 @@
       <c r="A94" s="0" t="s">
         <v>2083</v>
       </c>
-      <c r="B94" s="0" t="s">
+      <c r="B94" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C94" s="0" t="s">
         <v>2500</v>
       </c>
     </row>
@@ -33903,7 +33885,10 @@
       <c r="A95" s="0" t="s">
         <v>2084</v>
       </c>
-      <c r="B95" s="0" t="s">
+      <c r="B95" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C95" s="0" t="s">
         <v>2500</v>
       </c>
     </row>
@@ -33911,291 +33896,329 @@
       <c r="A96" s="0" t="s">
         <v>2085</v>
       </c>
-      <c r="B96" s="0" t="s">
+      <c r="B96" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C96" s="0" t="s">
         <v>2500</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>2086</v>
       </c>
-      <c r="B97" s="0" t="s">
+      <c r="B97" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C97" s="0" t="s">
         <v>2501</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>2087</v>
       </c>
-      <c r="B98" s="0" t="s">
+      <c r="B98" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C98" s="0" t="s">
         <v>2502</v>
       </c>
-      <c r="C98" s="0" t="s">
-        <v>2503</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>2088</v>
       </c>
-      <c r="B99" s="0" t="s">
-        <v>2504</v>
+      <c r="B99" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>2505</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2503</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>2089</v>
       </c>
-      <c r="B100" s="0" t="s">
-        <v>2506</v>
+      <c r="B100" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>2507</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2504</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>2090</v>
       </c>
-      <c r="B101" s="0" t="s">
-        <v>2508</v>
+      <c r="B101" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>2509</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2505</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>2092</v>
       </c>
-      <c r="B102" s="0" t="s">
-        <v>2510</v>
+      <c r="B102" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>2511</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2506</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>2093</v>
       </c>
-      <c r="B103" s="0" t="s">
-        <v>2512</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>2507</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>2094</v>
       </c>
-      <c r="B104" s="0" t="s">
-        <v>2513</v>
+      <c r="B104" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>2514</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2508</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>2095</v>
       </c>
-      <c r="B105" s="0" t="s">
-        <v>2515</v>
+      <c r="B105" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>2516</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2509</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>2097</v>
       </c>
-      <c r="B106" s="0" t="s">
-        <v>2517</v>
+      <c r="B106" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>2518</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2510</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>2098</v>
       </c>
-      <c r="B107" s="0" t="s">
-        <v>2519</v>
+      <c r="B107" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>2520</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2511</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
         <v>2099</v>
       </c>
-      <c r="B108" s="0" t="s">
-        <v>2521</v>
+      <c r="B108" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>2522</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2512</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>2100</v>
       </c>
-      <c r="B109" s="0" t="s">
-        <v>2523</v>
+      <c r="B109" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>2524</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2513</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>2101</v>
       </c>
-      <c r="B110" s="0" t="s">
-        <v>2525</v>
+      <c r="B110" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>2526</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2514</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>2102</v>
       </c>
-      <c r="B111" s="0" t="s">
-        <v>2527</v>
+      <c r="B111" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>2528</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2515</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>2103</v>
       </c>
-      <c r="B112" s="0" t="s">
-        <v>2529</v>
+      <c r="B112" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>2530</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2516</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>2104</v>
       </c>
-      <c r="B113" s="0" t="s">
-        <v>2531</v>
+      <c r="B113" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>2532</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2517</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
         <v>2106</v>
       </c>
-      <c r="B114" s="0" t="s">
-        <v>2533</v>
+      <c r="B114" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>2534</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2518</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
+        <v>2117</v>
+      </c>
+      <c r="B115" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>2519</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
         <v>2109</v>
       </c>
-      <c r="B115" s="0" t="s">
-        <v>2535</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
+      <c r="B117" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
         <v>2111</v>
       </c>
-      <c r="B116" s="0" t="s">
-        <v>2536</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="13" t="s">
+      <c r="B118" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>2521</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="13" t="s">
         <v>2113</v>
       </c>
-      <c r="B117" s="0" t="s">
-        <v>2537</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="s">
+      <c r="B119" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>2522</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
         <v>2114</v>
       </c>
-      <c r="B118" s="0" t="s">
-        <v>2538</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
-        <v>2117</v>
-      </c>
-      <c r="B119" s="0" t="s">
-        <v>2539</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="s">
+      <c r="B120" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>2523</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
         <v>2118</v>
       </c>
-      <c r="B120" s="0" t="s">
-        <v>2540</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="s">
+      <c r="B121" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>2524</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
         <v>2119</v>
       </c>
-      <c r="B121" s="0" t="s">
-        <v>2541</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
+      <c r="B122" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>2525</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
         <v>2120</v>
       </c>
-      <c r="B122" s="0" t="s">
-        <v>2542</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="13" t="s">
+      <c r="B123" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>2526</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="13" t="s">
         <v>2121</v>
       </c>
-      <c r="B123" s="0" t="s">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
+      <c r="B124" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
         <v>2122</v>
       </c>
-      <c r="B124" s="0" t="s">
-        <v>2544</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="s">
+      <c r="B125" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C125" s="0" t="s">
+        <v>2528</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
         <v>2127</v>
       </c>
-      <c r="B125" s="0" t="s">
-        <v>2545</v>
-      </c>
-    </row>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C126" s="0" t="s">
+        <v>2529</v>
+      </c>
+    </row>
     <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -34230,7 +34253,7 @@
   </sheetPr>
   <dimension ref="A1:W106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H71" activeCellId="0" sqref="H71"/>
     </sheetView>
   </sheetViews>
@@ -34249,13 +34272,13 @@
         <v>1506</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>2546</v>
+        <v>2530</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>2547</v>
+        <v>2531</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>2548</v>
+        <v>2532</v>
       </c>
       <c r="I2" s="0" t="str">
         <f aca="false">CONCATENATE(E2,A2,G2, B2, ".unique")</f>
@@ -34325,7 +34348,7 @@
         <v>1611</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>2549</v>
+        <v>2533</v>
       </c>
       <c r="W9" s="1"/>
     </row>
@@ -34769,13 +34792,13 @@
         <v>314</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>2546</v>
+        <v>2530</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>2550</v>
+        <v>2534</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>2548</v>
+        <v>2532</v>
       </c>
       <c r="I63" s="0" t="str">
         <f aca="false">CONCATENATE(E63,A63,G63, B63, ".unique")</f>
@@ -34798,7 +34821,7 @@
         <v>298</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>2551</v>
+        <v>2535</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35162,13 +35185,13 @@
         <v>2</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>2552</v>
+        <v>2536</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2553</v>
+        <v>2537</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>2554</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35179,10 +35202,10 @@
         <v>1275</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>2555</v>
+        <v>2539</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>2556</v>
+        <v>2540</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1276</v>
@@ -35196,10 +35219,10 @@
         <v>1426</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>2557</v>
+        <v>2541</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>2557</v>
+        <v>2541</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1427</v>
@@ -35213,10 +35236,10 @@
         <v>1922</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>2558</v>
+        <v>2542</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>2559</v>
+        <v>2543</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>1923</v>
@@ -35230,10 +35253,10 @@
         <v>1928</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>2560</v>
+        <v>2544</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>2561</v>
+        <v>2545</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>1929</v>
@@ -35247,10 +35270,10 @@
         <v>1934</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>2562</v>
+        <v>2546</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>2563</v>
+        <v>2547</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>1935</v>
@@ -35264,10 +35287,10 @@
         <v>1940</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>2564</v>
+        <v>2548</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>2565</v>
+        <v>2549</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>1941</v>
@@ -35281,10 +35304,10 @@
         <v>1917</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>2566</v>
+        <v>2550</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>2567</v>
+        <v>2551</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>1918</v>
@@ -35298,10 +35321,10 @@
         <v>1908</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>2568</v>
+        <v>2552</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>2569</v>
+        <v>2553</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>1909</v>
@@ -35315,10 +35338,10 @@
         <v>49</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>2570</v>
+        <v>2554</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>2571</v>
+        <v>2555</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>50</v>
@@ -35332,10 +35355,10 @@
         <v>58</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>2572</v>
+        <v>2556</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>2573</v>
+        <v>2557</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>59</v>
@@ -35349,10 +35372,10 @@
         <v>66</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>2574</v>
+        <v>2558</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>2575</v>
+        <v>2559</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>67</v>
@@ -35366,10 +35389,10 @@
         <v>73</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>2576</v>
+        <v>2560</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>2577</v>
+        <v>2561</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>74</v>
@@ -35383,10 +35406,10 @@
         <v>81</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>2578</v>
+        <v>2562</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>2579</v>
+        <v>2563</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>82</v>
@@ -35400,10 +35423,10 @@
         <v>88</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>2580</v>
+        <v>2564</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>2581</v>
+        <v>2565</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>89</v>
@@ -35417,10 +35440,10 @@
         <v>97</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>2582</v>
+        <v>2566</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>2583</v>
+        <v>2567</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>98</v>
@@ -35434,10 +35457,10 @@
         <v>119</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>2584</v>
+        <v>2568</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>2585</v>
+        <v>2569</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>120</v>
@@ -35451,10 +35474,10 @@
         <v>128</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>2586</v>
+        <v>2570</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>2587</v>
+        <v>2571</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>129</v>
@@ -35468,10 +35491,10 @@
         <v>136</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>2588</v>
+        <v>2572</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>2589</v>
+        <v>2573</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>137</v>
@@ -35485,10 +35508,10 @@
         <v>159</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>2590</v>
+        <v>2574</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>2591</v>
+        <v>2575</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>160</v>
@@ -35502,10 +35525,10 @@
         <v>175</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>2592</v>
+        <v>2576</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>2593</v>
+        <v>2577</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>176</v>
@@ -35519,10 +35542,10 @@
         <v>227</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>2594</v>
+        <v>2578</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>2595</v>
+        <v>2579</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>228</v>
@@ -35536,10 +35559,10 @@
         <v>237</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>2596</v>
+        <v>2580</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>2597</v>
+        <v>2581</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>238</v>
@@ -35553,10 +35576,10 @@
         <v>255</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>2598</v>
+        <v>2582</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>2599</v>
+        <v>2583</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>256</v>
@@ -35570,10 +35593,10 @@
         <v>271</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>2600</v>
+        <v>2584</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>2601</v>
+        <v>2585</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>272</v>
@@ -35587,10 +35610,10 @@
         <v>369</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>2602</v>
+        <v>2586</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>2603</v>
+        <v>2587</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>370</v>
@@ -35604,10 +35627,10 @@
         <v>436</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>2604</v>
+        <v>2588</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>2605</v>
+        <v>2589</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>437</v>
@@ -35621,10 +35644,10 @@
         <v>442</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>2606</v>
+        <v>2590</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>2607</v>
+        <v>2591</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>443</v>
@@ -35638,10 +35661,10 @@
         <v>450</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>2608</v>
+        <v>2592</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>2609</v>
+        <v>2593</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>451</v>
@@ -35655,10 +35678,10 @@
         <v>459</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>2610</v>
+        <v>2594</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>2611</v>
+        <v>2595</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>460</v>
@@ -35672,10 +35695,10 @@
         <v>467</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>2612</v>
+        <v>2596</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>2613</v>
+        <v>2597</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>468</v>
@@ -35689,10 +35712,10 @@
         <v>475</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>2614</v>
+        <v>2598</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>2615</v>
+        <v>2599</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>476</v>
@@ -35706,10 +35729,10 @@
         <v>484</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>2616</v>
+        <v>2600</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>2617</v>
+        <v>2601</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>485</v>
@@ -35723,10 +35746,10 @@
         <v>493</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>2618</v>
+        <v>2602</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>2619</v>
+        <v>2603</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>494</v>
@@ -35740,10 +35763,10 @@
         <v>501</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>2620</v>
+        <v>2604</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>2621</v>
+        <v>2605</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>502</v>
@@ -35757,10 +35780,10 @@
         <v>517</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>2622</v>
+        <v>2606</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>2623</v>
+        <v>2607</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>518</v>
@@ -35774,10 +35797,10 @@
         <v>550</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>2624</v>
+        <v>2608</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>2625</v>
+        <v>2609</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>551</v>
@@ -35791,10 +35814,10 @@
         <v>558</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>2626</v>
+        <v>2610</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>2627</v>
+        <v>2611</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>559</v>
@@ -35808,10 +35831,10 @@
         <v>566</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>2628</v>
+        <v>2612</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>2629</v>
+        <v>2613</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>567</v>
@@ -35825,10 +35848,10 @@
         <v>574</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>2630</v>
+        <v>2614</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>2631</v>
+        <v>2615</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>575</v>
@@ -35842,10 +35865,10 @@
         <v>582</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>2632</v>
+        <v>2616</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>2633</v>
+        <v>2617</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>583</v>
@@ -35859,10 +35882,10 @@
         <v>590</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>2634</v>
+        <v>2618</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>2635</v>
+        <v>2619</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>591</v>
@@ -35876,10 +35899,10 @@
         <v>635</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>2636</v>
+        <v>2620</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>2637</v>
+        <v>2621</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>636</v>
@@ -35893,10 +35916,10 @@
         <v>700</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>2638</v>
+        <v>2622</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>2639</v>
+        <v>2623</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>701</v>
@@ -35910,10 +35933,10 @@
         <v>708</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>2640</v>
+        <v>2624</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>2641</v>
+        <v>2625</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>709</v>
@@ -35927,10 +35950,10 @@
         <v>723</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>2642</v>
+        <v>2626</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>2643</v>
+        <v>2627</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>724</v>
@@ -35944,10 +35967,10 @@
         <v>731</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>2644</v>
+        <v>2628</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>2645</v>
+        <v>2629</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>732</v>
@@ -35961,10 +35984,10 @@
         <v>756</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>2646</v>
+        <v>2630</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>2647</v>
+        <v>2631</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>757</v>
@@ -35978,10 +36001,10 @@
         <v>764</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>2648</v>
+        <v>2632</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>2649</v>
+        <v>2633</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>765</v>
@@ -35995,10 +36018,10 @@
         <v>772</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>2650</v>
+        <v>2634</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>2651</v>
+        <v>2635</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>773</v>
@@ -36012,10 +36035,10 @@
         <v>806</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>2652</v>
+        <v>2636</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>2653</v>
+        <v>2637</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>807</v>
@@ -36029,10 +36052,10 @@
         <v>814</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>2654</v>
+        <v>2638</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>2655</v>
+        <v>2639</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>815</v>
@@ -36046,10 +36069,10 @@
         <v>855</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>2656</v>
+        <v>2640</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>2657</v>
+        <v>2641</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>856</v>
@@ -36063,10 +36086,10 @@
         <v>944</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>2658</v>
+        <v>2642</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>2659</v>
+        <v>2643</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>945</v>
@@ -36080,10 +36103,10 @@
         <v>962</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>2660</v>
+        <v>2644</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>2661</v>
+        <v>2645</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>963</v>
@@ -36097,10 +36120,10 @@
         <v>971</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>2662</v>
+        <v>2646</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>2663</v>
+        <v>2647</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>972</v>
@@ -36114,10 +36137,10 @@
         <v>988</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>2664</v>
+        <v>2648</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>2665</v>
+        <v>2649</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>989</v>
@@ -36131,10 +36154,10 @@
         <v>995</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>2666</v>
+        <v>2650</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>2667</v>
+        <v>2651</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>996</v>
@@ -36148,10 +36171,10 @@
         <v>1004</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>2668</v>
+        <v>2652</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>2669</v>
+        <v>2653</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>1005</v>
@@ -36165,10 +36188,10 @@
         <v>1012</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>2670</v>
+        <v>2654</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>2671</v>
+        <v>2655</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>1013</v>
@@ -36182,10 +36205,10 @@
         <v>1021</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>2672</v>
+        <v>2656</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>2673</v>
+        <v>2657</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>1022</v>
@@ -36199,10 +36222,10 @@
         <v>1029</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>2674</v>
+        <v>2658</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>2675</v>
+        <v>2659</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>1030</v>
@@ -36216,10 +36239,10 @@
         <v>1039</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>2676</v>
+        <v>2660</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>2677</v>
+        <v>2661</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>1040</v>
@@ -36233,10 +36256,10 @@
         <v>1046</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>2678</v>
+        <v>2662</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>2679</v>
+        <v>2663</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>1047</v>
@@ -36250,10 +36273,10 @@
         <v>1053</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>2680</v>
+        <v>2664</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>2681</v>
+        <v>2665</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>1054</v>
@@ -36267,10 +36290,10 @@
         <v>1060</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>2682</v>
+        <v>2666</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>2683</v>
+        <v>2667</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>1061</v>
@@ -36284,10 +36307,10 @@
         <v>1068</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>2684</v>
+        <v>2668</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>2685</v>
+        <v>2669</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>1069</v>
@@ -36301,10 +36324,10 @@
         <v>1077</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>2686</v>
+        <v>2670</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>2687</v>
+        <v>2671</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>1078</v>
@@ -36318,10 +36341,10 @@
         <v>1086</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>2688</v>
+        <v>2672</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>2689</v>
+        <v>2673</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>1087</v>
@@ -36335,10 +36358,10 @@
         <v>1096</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>2690</v>
+        <v>2674</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>2691</v>
+        <v>2675</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>1097</v>
@@ -36352,10 +36375,10 @@
         <v>1105</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>2692</v>
+        <v>2676</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>2693</v>
+        <v>2677</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>1106</v>
@@ -36369,10 +36392,10 @@
         <v>1114</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>2694</v>
+        <v>2678</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>2695</v>
+        <v>2679</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>1115</v>
@@ -36386,10 +36409,10 @@
         <v>1123</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>2696</v>
+        <v>2680</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>2697</v>
+        <v>2681</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>1124</v>
@@ -36403,10 +36426,10 @@
         <v>1147</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>2698</v>
+        <v>2682</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>2699</v>
+        <v>2683</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>1148</v>
@@ -36420,10 +36443,10 @@
         <v>1172</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>2700</v>
+        <v>2684</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>2701</v>
+        <v>2685</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>1173</v>
@@ -36437,10 +36460,10 @@
         <v>1187</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>2702</v>
+        <v>2686</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>2703</v>
+        <v>2687</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>1188</v>
@@ -36454,10 +36477,10 @@
         <v>1195</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>2704</v>
+        <v>2688</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>2705</v>
+        <v>2689</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>1196</v>
@@ -36471,10 +36494,10 @@
         <v>1203</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>2706</v>
+        <v>2690</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>2707</v>
+        <v>2691</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>1204</v>
@@ -36488,10 +36511,10 @@
         <v>1212</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>2708</v>
+        <v>2692</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>2709</v>
+        <v>2693</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>1213</v>
@@ -36505,10 +36528,10 @@
         <v>1219</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>2710</v>
+        <v>2694</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>2711</v>
+        <v>2695</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>1220</v>
@@ -36522,10 +36545,10 @@
         <v>1226</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>2712</v>
+        <v>2696</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>2713</v>
+        <v>2697</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>1227</v>
@@ -36539,10 +36562,10 @@
         <v>1235</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>2714</v>
+        <v>2698</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>2715</v>
+        <v>2699</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>1236</v>
@@ -36556,10 +36579,10 @@
         <v>1243</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>2716</v>
+        <v>2700</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>2717</v>
+        <v>2701</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>1244</v>
@@ -36573,10 +36596,10 @@
         <v>1252</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>2718</v>
+        <v>2702</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>2719</v>
+        <v>2703</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>1253</v>
@@ -36590,10 +36613,10 @@
         <v>1259</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>2720</v>
+        <v>2704</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>2721</v>
+        <v>2705</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>1260</v>
@@ -36607,10 +36630,10 @@
         <v>1284</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>2722</v>
+        <v>2706</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>2723</v>
+        <v>2707</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>1285</v>
@@ -36624,10 +36647,10 @@
         <v>1293</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>2724</v>
+        <v>2708</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>2725</v>
+        <v>2709</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>1294</v>
@@ -36641,10 +36664,10 @@
         <v>1302</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>2726</v>
+        <v>2710</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>2727</v>
+        <v>2711</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>1303</v>
@@ -36658,10 +36681,10 @@
         <v>1309</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>2728</v>
+        <v>2712</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>2729</v>
+        <v>2713</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>1310</v>
@@ -36675,10 +36698,10 @@
         <v>1316</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>2730</v>
+        <v>2714</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>2731</v>
+        <v>2715</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>1317</v>
@@ -36692,10 +36715,10 @@
         <v>1323</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>2732</v>
+        <v>2716</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>2733</v>
+        <v>2717</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>1324</v>
@@ -36709,10 +36732,10 @@
         <v>1332</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>2734</v>
+        <v>2718</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>2735</v>
+        <v>2719</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>1333</v>
@@ -36726,10 +36749,10 @@
         <v>1339</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>2736</v>
+        <v>2720</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>2737</v>
+        <v>2721</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>1340</v>
@@ -36743,10 +36766,10 @@
         <v>1347</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>2738</v>
+        <v>2722</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>2739</v>
+        <v>2723</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>1348</v>
@@ -36760,10 +36783,10 @@
         <v>1356</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>2740</v>
+        <v>2724</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>2741</v>
+        <v>2725</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>1357</v>
@@ -36777,10 +36800,10 @@
         <v>1371</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>2742</v>
+        <v>2726</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>2743</v>
+        <v>2727</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>1372</v>
@@ -36794,10 +36817,10 @@
         <v>1380</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>2744</v>
+        <v>2728</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>2745</v>
+        <v>2729</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>1381</v>
@@ -36811,10 +36834,10 @@
         <v>1388</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>2746</v>
+        <v>2730</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>2747</v>
+        <v>2731</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>1389</v>
@@ -36828,10 +36851,10 @@
         <v>1396</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>2748</v>
+        <v>2732</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>2749</v>
+        <v>2733</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>1397</v>
@@ -36845,10 +36868,10 @@
         <v>1403</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>2750</v>
+        <v>2734</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>2751</v>
+        <v>2735</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>1404</v>
@@ -36862,10 +36885,10 @@
         <v>1411</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>2752</v>
+        <v>2736</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>2753</v>
+        <v>2737</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>1412</v>
@@ -36879,10 +36902,10 @@
         <v>1418</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>2754</v>
+        <v>2738</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>2755</v>
+        <v>2739</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>1419</v>
@@ -36896,10 +36919,10 @@
         <v>1450</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>2756</v>
+        <v>2740</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>2757</v>
+        <v>2741</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>1451</v>
@@ -36913,10 +36936,10 @@
         <v>1473</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>2758</v>
+        <v>2742</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>2759</v>
+        <v>2743</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>1474</v>
@@ -36930,10 +36953,10 @@
         <v>1481</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>2760</v>
+        <v>2744</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>2761</v>
+        <v>2745</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>1482</v>
@@ -36947,10 +36970,10 @@
         <v>1569</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>2762</v>
+        <v>2746</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>2763</v>
+        <v>2747</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>1570</v>
@@ -36964,10 +36987,10 @@
         <v>1602</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>2764</v>
+        <v>2748</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>2765</v>
+        <v>2749</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>1603</v>
@@ -36981,10 +37004,10 @@
         <v>1625</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>2766</v>
+        <v>2750</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>2767</v>
+        <v>2751</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>1626</v>
@@ -36998,10 +37021,10 @@
         <v>1633</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>2768</v>
+        <v>2752</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>2769</v>
+        <v>2753</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>1634</v>
@@ -37015,10 +37038,10 @@
         <v>1643</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>2770</v>
+        <v>2754</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>2771</v>
+        <v>2755</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>1644</v>
@@ -37032,10 +37055,10 @@
         <v>1666</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>2772</v>
+        <v>2756</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>2773</v>
+        <v>2757</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>1667</v>
@@ -37049,10 +37072,10 @@
         <v>1683</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>2774</v>
+        <v>2758</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>2775</v>
+        <v>2759</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>1684</v>
@@ -37066,10 +37089,10 @@
         <v>1734</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>2776</v>
+        <v>2760</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>2777</v>
+        <v>2761</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>1735</v>
@@ -37083,10 +37106,10 @@
         <v>1742</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>2778</v>
+        <v>2762</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>2779</v>
+        <v>2763</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>1743</v>
@@ -37100,10 +37123,10 @@
         <v>1759</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>2780</v>
+        <v>2764</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>2781</v>
+        <v>2765</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>1760</v>
@@ -37117,10 +37140,10 @@
         <v>1768</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>2782</v>
+        <v>2766</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>2783</v>
+        <v>2767</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>1769</v>
@@ -37134,10 +37157,10 @@
         <v>1785</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>2784</v>
+        <v>2768</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>2785</v>
+        <v>2769</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>1786</v>
@@ -37151,10 +37174,10 @@
         <v>1811</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>2786</v>
+        <v>2770</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>2787</v>
+        <v>2771</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>1812</v>
@@ -37168,10 +37191,10 @@
         <v>1827</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>2788</v>
+        <v>2772</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>2789</v>
+        <v>2773</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>1828</v>
@@ -37185,10 +37208,10 @@
         <v>1835</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>2790</v>
+        <v>2774</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>2791</v>
+        <v>2775</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>1836</v>
@@ -37202,10 +37225,10 @@
         <v>1842</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>2792</v>
+        <v>2776</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>2793</v>
+        <v>2777</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>1843</v>
@@ -37219,10 +37242,10 @@
         <v>1850</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>2794</v>
+        <v>2778</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>2795</v>
+        <v>2779</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>1851</v>
@@ -37236,10 +37259,10 @@
         <v>1858</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>2796</v>
+        <v>2780</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>2797</v>
+        <v>2781</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>1859</v>
@@ -37253,10 +37276,10 @@
         <v>1874</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>2798</v>
+        <v>2782</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>2799</v>
+        <v>2783</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>1875</v>
@@ -37270,10 +37293,10 @@
         <v>741</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>2800</v>
+        <v>2784</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>2801</v>
+        <v>2785</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>742</v>
@@ -37287,10 +37310,10 @@
         <v>797</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>2802</v>
+        <v>2786</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>2803</v>
+        <v>2787</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>798</v>
@@ -37304,10 +37327,10 @@
         <v>1750</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>2804</v>
+        <v>2788</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>2805</v>
+        <v>2789</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>1751</v>
@@ -37321,10 +37344,10 @@
         <v>1651</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>2806</v>
+        <v>2790</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>2807</v>
+        <v>2791</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>1652</v>
@@ -37338,10 +37361,10 @@
         <v>599</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>2808</v>
+        <v>2792</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>2809</v>
+        <v>2793</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>600</v>

</xml_diff>